<commit_message>
1 - Achiz 2022
</commit_message>
<xml_diff>
--- a/main/Nr.1 Apeducte-Canalizare/tab_2019_tab1_tab1.xlsx
+++ b/main/Nr.1 Apeducte-Canalizare/tab_2019_tab1_tab1.xlsx
@@ -41,7 +41,7 @@
     <t>TAB_1_COL_3</t>
   </si>
   <si>
-    <t>TAB_1_COL_4</t>
+    <t>TAB_1_COL_7</t>
   </si>
   <si>
     <t>TAB_1_1_COL_12</t>
@@ -185,7 +185,7 @@
     <t>S.CIORESCU</t>
   </si>
   <si>
-    <t>0152</t>
+    <t>1003600115544</t>
   </si>
   <si>
     <t>INTREPRINDERE MUNICIPALA REGIA COMUNAL-LOCATIVA CIORESCU""</t>
@@ -431,7 +431,7 @@
     <t>OR.DONDUSENI</t>
   </si>
   <si>
-    <t>3446</t>
+    <t>1004604000366</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA APA-CANAL DONDUSENI""</t>
@@ -827,7 +827,7 @@
     <t>OR.CUPCINI</t>
   </si>
   <si>
-    <t>4102</t>
+    <t>1018620002156</t>
   </si>
   <si>
     <t>INSTITUTIA PUBLICA SCOALA PROFESIONALA,OR.CUPCINI,R-UL EDINET</t>
@@ -872,7 +872,7 @@
     <t>S.BRATUSENI</t>
   </si>
   <si>
-    <t>4114</t>
+    <t>1003604007690</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA "GOSPODARIA COMUNALA SI DE LOCUINTE A SATULUI BRATUSENI"</t>
@@ -1016,7 +1016,7 @@
     <t>OR.FALESTI</t>
   </si>
   <si>
-    <t>4301</t>
+    <t>1004602005437</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA DIRECTIA DE PRODUCTIE A GOSPODARIEI COMUNALE SI DE LOCUINTE DIN OR.FALESTI""</t>
@@ -1505,7 +1505,7 @@
     <t>OR.GLODENI</t>
   </si>
   <si>
-    <t>4801</t>
+    <t>1008602006801</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA SERVICII COMUNALE GLODENI""</t>
@@ -1781,7 +1781,7 @@
     <t>OR.FRUNZA</t>
   </si>
   <si>
-    <t>6202</t>
+    <t>1003604014092</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA DIRECTIA GOSPODARIEI LOCATIV-COMUNALE FRUNZA""</t>
@@ -1796,7 +1796,7 @@
     <t>OR.OTACI</t>
   </si>
   <si>
-    <t>6203</t>
+    <t>1005604001809</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA GOSPODARIA LOCATIV-COMUNALA OTACI""</t>
@@ -1835,7 +1835,7 @@
     <t>OR.COSTESTI</t>
   </si>
   <si>
-    <t>7122</t>
+    <t>1003602151865</t>
   </si>
   <si>
     <t>Intreprinderea Municipala Directia de Productie "APA-CANAL" COSTESTI</t>
@@ -2216,7 +2216,7 @@
     <t>OR.BIRUINTA</t>
   </si>
   <si>
-    <t>7402</t>
+    <t>1005602001779</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA DIRECTIA DE PRODUCTIE A GOSPODARIEI COMUNALE - LOCATIVE DIN BIRUINTA""</t>
@@ -2900,7 +2900,7 @@
     <t>S.MAXIMOVCA</t>
   </si>
   <si>
-    <t>1032</t>
+    <t>1007600046332</t>
   </si>
   <si>
     <t>Intreprinderea Municipala "MAXIMOVCA - ACVA"</t>
@@ -3005,7 +3005,7 @@
     <t>S.SPEIA</t>
   </si>
   <si>
-    <t>1041</t>
+    <t>1003601002214</t>
   </si>
   <si>
     <t>Intreprinderea Municipala "INTREPRINDEREA INTERCOMUNITARA DE UTILITATI PUBLICE SPEIA"</t>
@@ -3092,7 +3092,7 @@
     <t>OR.CALARASI</t>
   </si>
   <si>
-    <t>2501</t>
+    <t>1003609007259</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA GOSPODARIA COMUNAL-LOCATIVA CALARASI""</t>
@@ -3398,7 +3398,7 @@
     <t>OR.CRIULENI</t>
   </si>
   <si>
-    <t>3101</t>
+    <t>1004600033580</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA COMUNSERVICE" CRIULENI"</t>
@@ -4196,7 +4196,7 @@
     <t>S.PERENI</t>
   </si>
   <si>
-    <t>33326659</t>
+    <t>1021620005724</t>
   </si>
   <si>
     <t>ASOCIATIA OBSTEASCA A CONSUMATORILOR DE APA "SIPOTEL"</t>
@@ -4673,7 +4673,7 @@
     <t>S.BALANESTI</t>
   </si>
   <si>
-    <t>36987714</t>
+    <t>1022620012488</t>
   </si>
   <si>
     <t>ASOCIATIA OBSTEASCA ASOCIATIA UTILIZATORILOR DE APA BALANESTI</t>
@@ -5207,7 +5207,7 @@
     <t>ASOCIATIA UTILIZATORILOR DE APA "HODOLINA"</t>
   </si>
   <si>
-    <t>35363745</t>
+    <t>1022620007884</t>
   </si>
   <si>
     <t>ASOCIATIA UTILIZATORILOR DE APA SI CANALIZARE "CRISCA"</t>
@@ -5438,7 +5438,7 @@
     <t>S.ZORILE</t>
   </si>
   <si>
-    <t>32052742</t>
+    <t>1021620000420</t>
   </si>
   <si>
     <t>ASOCIATIA OBSTEASCA "APA VIE"</t>
@@ -5462,7 +5462,7 @@
     <t>OR.REZINA</t>
   </si>
   <si>
-    <t>6701</t>
+    <t>1003606012829</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA SERVICII COMUNAL-LOCATIVE" REZINA"</t>
@@ -5888,7 +5888,7 @@
     <t>OR.SOLDANESTI</t>
   </si>
   <si>
-    <t>8301</t>
+    <t>1007606005218</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA REGIA APA SOLDANESTI" IN PROCES DE INSOLVABILITATE"</t>
@@ -6830,7 +6830,7 @@
     <t>S.ALEXANDERFELD</t>
   </si>
   <si>
-    <t>9414</t>
+    <t>1002603000435</t>
   </si>
   <si>
     <t>COOPERATIVA AGRICOLA DE PRODUCTIE PENTRU PRODUCEREA SEMINTELOR "ELITA-ALEXANDERFELD"</t>
@@ -7226,7 +7226,7 @@
     <t>OR.CANTEMIR</t>
   </si>
   <si>
-    <t>2101</t>
+    <t>1004603000897</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA APA-CANAL CANTEMIR""</t>
@@ -7292,7 +7292,7 @@
     <t>Intreprinderea Municipala "CIOBALACCIA-SERVICII"</t>
   </si>
   <si>
-    <t>2119</t>
+    <t>1002603000181</t>
   </si>
   <si>
     <t>Cooperativa Agricola de Productie "CIOBALACCIA"</t>
@@ -7976,7 +7976,7 @@
     <t>OR.CIMISLIA</t>
   </si>
   <si>
-    <t>2901</t>
+    <t>1011605000455</t>
   </si>
   <si>
     <t>INTREPRINDEREA MUNICIPALA SERVICII PUBLICE CIMISLIA""</t>

</xml_diff>